<commit_message>
2016-10-15:mission objectives, user views refactored
</commit_message>
<xml_diff>
--- a/project_manual/user views.xlsx
+++ b/project_manual/user views.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="17">
   <si>
     <t>Professor</t>
   </si>
@@ -63,7 +63,10 @@
     <t>x</t>
   </si>
   <si>
-    <t>x?</t>
+    <t>data on services provided to another faculty</t>
+  </si>
+  <si>
+    <t>data on services used from another faculty</t>
   </si>
 </sst>
 </file>
@@ -491,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:G17"/>
+  <dimension ref="B2:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,9 +536,7 @@
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>14</v>
@@ -547,9 +548,7 @@
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5" t="s">
         <v>14</v>
@@ -579,9 +578,7 @@
       <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
         <v>14</v>
@@ -593,9 +590,7 @@
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
         <v>14</v>
@@ -636,9 +631,7 @@
         <v>7</v>
       </c>
       <c r="D10" s="5"/>
-      <c r="E10" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
         <v>14</v>
       </c>
@@ -680,9 +673,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E13" s="5"/>
       <c r="F13" s="5" t="s">
         <v>14</v>
       </c>
@@ -709,9 +700,7 @@
       <c r="C15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
         <v>14</v>
@@ -723,9 +712,7 @@
       <c r="C16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>14</v>
-      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5" t="s">
         <v>14</v>
@@ -747,6 +734,90 @@
         <v>14</v>
       </c>
       <c r="G17" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
+      <c r="C19" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19" s="6"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="6"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="7"/>
+      <c r="C23" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="9" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>